<commit_message>
Added highest score variables
I have added the highest GCSE points score variables alongside the highest A*-C grades in the 18 main subjects
</commit_message>
<xml_diff>
--- a/ycs_background_variables.xlsx
+++ b/ycs_background_variables.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="142">
   <si>
     <t>variable number</t>
   </si>
@@ -105,6 +105,18 @@
     <t>t0mumsoc</t>
   </si>
   <si>
+    <t>t0examst</t>
+  </si>
+  <si>
+    <t>t0examac</t>
+  </si>
+  <si>
+    <t>t0examaf</t>
+  </si>
+  <si>
+    <t>t0score</t>
+  </si>
+  <si>
     <t>t0dadse</t>
   </si>
   <si>
@@ -238,6 +250,18 @@
   </si>
   <si>
     <t>SOC90 code of mothers’ occupation</t>
+  </si>
+  <si>
+    <t>num of y11 exam courses studied</t>
+  </si>
+  <si>
+    <t>num of a-c awards in y11 or s4 exams</t>
+  </si>
+  <si>
+    <t>num of a-f awards in y11 or s4 exams</t>
+  </si>
+  <si>
+    <t>point score from y11 or s4 exams</t>
   </si>
   <si>
     <t>is/was your father self-employed?</t>
@@ -471,19 +495,19 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="F1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="G1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2">
@@ -494,19 +518,19 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D2" s="0">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3">
@@ -517,19 +541,19 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D3" s="0">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F3" t="s">
         <v>3</v>
       </c>
       <c r="G3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4">
@@ -540,19 +564,19 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D4" s="0">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F4" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G4" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5">
@@ -563,19 +587,19 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D5" s="0">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F5" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G5" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6">
@@ -586,19 +610,19 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D6" s="0">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G6" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7">
@@ -609,19 +633,19 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D7" s="0">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="F7" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G7" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8">
@@ -632,19 +656,19 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D8" s="0">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="F8" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G8" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9">
@@ -655,19 +679,19 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D9" s="0">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F9" t="s">
         <v>9</v>
       </c>
       <c r="G9" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10">
@@ -678,19 +702,19 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D10" s="0">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F10" t="s">
         <v>10</v>
       </c>
       <c r="G10" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11">
@@ -701,19 +725,19 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D11" s="0">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F11" t="s">
         <v>11</v>
       </c>
       <c r="G11" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12">
@@ -724,19 +748,19 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D12" s="0">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F12" t="s">
         <v>12</v>
       </c>
       <c r="G12" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13">
@@ -747,19 +771,19 @@
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D13" s="0">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F13" t="s">
         <v>13</v>
       </c>
       <c r="G13" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14">
@@ -770,19 +794,19 @@
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D14" s="0">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F14" t="s">
         <v>14</v>
       </c>
       <c r="G14" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15">
@@ -793,19 +817,19 @@
         <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D15" s="0">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F15" t="s">
         <v>15</v>
       </c>
       <c r="G15" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16">
@@ -816,19 +840,19 @@
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D16" s="0">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F16" t="s">
         <v>16</v>
       </c>
       <c r="G16" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17">
@@ -839,19 +863,19 @@
         <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D17" s="0">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F17" t="s">
         <v>17</v>
       </c>
       <c r="G17" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18">
@@ -862,19 +886,19 @@
         <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D18" s="0">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F18" t="s">
         <v>18</v>
       </c>
       <c r="G18" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19">
@@ -885,19 +909,19 @@
         <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D19" s="0">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F19" t="s">
         <v>19</v>
       </c>
       <c r="G19" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20">
@@ -908,19 +932,19 @@
         <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D20" s="0">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F20" t="s">
         <v>20</v>
       </c>
       <c r="G20" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21">
@@ -931,19 +955,19 @@
         <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D21" s="0">
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F21" t="s">
         <v>21</v>
       </c>
       <c r="G21" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22">
@@ -954,19 +978,19 @@
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D22" s="0">
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F22" t="s">
         <v>22</v>
       </c>
       <c r="G22" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23">
@@ -977,19 +1001,19 @@
         <v>23</v>
       </c>
       <c r="C23" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D23" s="0">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F23" t="s">
         <v>23</v>
       </c>
       <c r="G23" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24">
@@ -1000,19 +1024,19 @@
         <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D24" s="0">
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F24" t="s">
         <v>24</v>
       </c>
       <c r="G24" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25">
@@ -1023,19 +1047,19 @@
         <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D25" s="0">
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F25" t="s">
         <v>25</v>
       </c>
       <c r="G25" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26">
@@ -1046,19 +1070,19 @@
         <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D26" s="0">
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F26" t="s">
         <v>26</v>
       </c>
       <c r="G26" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27">
@@ -1069,19 +1093,19 @@
         <v>27</v>
       </c>
       <c r="C27" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D27" s="0">
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F27" t="s">
         <v>27</v>
       </c>
       <c r="G27" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28">
@@ -1092,19 +1116,19 @@
         <v>28</v>
       </c>
       <c r="C28" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D28" s="0">
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F28" t="s">
         <v>28</v>
       </c>
       <c r="G28" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29">
@@ -1115,19 +1139,19 @@
         <v>29</v>
       </c>
       <c r="C29" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D29" s="0">
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F29" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="G29" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30">
@@ -1138,19 +1162,19 @@
         <v>30</v>
       </c>
       <c r="C30" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D30" s="0">
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F30" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="G30" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31">
@@ -1161,19 +1185,111 @@
         <v>31</v>
       </c>
       <c r="C31" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="0">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" t="s">
+        <v>49</v>
+      </c>
+      <c r="G31" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" s="0">
+        <v>1</v>
+      </c>
+      <c r="E32" t="s">
+        <v>44</v>
+      </c>
+      <c r="F32" t="s">
+        <v>49</v>
+      </c>
+      <c r="G32" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33" s="0">
+        <v>1</v>
+      </c>
+      <c r="E33" t="s">
+        <v>44</v>
+      </c>
+      <c r="F33" t="s">
+        <v>33</v>
+      </c>
+      <c r="G33" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
         <v>34</v>
       </c>
-      <c r="D31" s="0">
-        <v>1</v>
-      </c>
-      <c r="E31" t="s">
-        <v>40</v>
-      </c>
-      <c r="F31" t="s">
-        <v>31</v>
-      </c>
-      <c r="G31" t="s">
-        <v>76</v>
+      <c r="C34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" s="0">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>44</v>
+      </c>
+      <c r="F34" t="s">
+        <v>34</v>
+      </c>
+      <c r="G34" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" s="0">
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
+        <v>44</v>
+      </c>
+      <c r="F35" t="s">
+        <v>35</v>
+      </c>
+      <c r="G35" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1192,19 +1308,19 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="F1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="G1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2">
@@ -1215,19 +1331,19 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D2" s="0">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3">
@@ -1238,19 +1354,19 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D3" s="0">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="F3" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="G3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4">
@@ -1261,19 +1377,19 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D4" s="0">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F4" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G4" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5">
@@ -1284,19 +1400,19 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="D5" s="0">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="F5" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G5" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6">
@@ -1307,19 +1423,19 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D6" s="0">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G6" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7">
@@ -1330,19 +1446,19 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D7" s="0">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="F7" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G7" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8">
@@ -1353,19 +1469,19 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D8" s="0">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="F8" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G8" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9">
@@ -1376,19 +1492,19 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D9" s="0">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="F9" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="G9" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10">
@@ -1399,19 +1515,19 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D10" s="0">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="F10" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="G10" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11">
@@ -1422,19 +1538,19 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D11" s="0">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="F11" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="G11" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12">
@@ -1445,19 +1561,19 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D12" s="0">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="F12" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="G12" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13">
@@ -1468,19 +1584,19 @@
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D13" s="0">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="F13" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="G13" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14">
@@ -1491,19 +1607,19 @@
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D14" s="0">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="F14" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="G14" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15">
@@ -1514,19 +1630,19 @@
         <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D15" s="0">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="F15" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="G15" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16">
@@ -1537,19 +1653,19 @@
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D16" s="0">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="F16" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="G16" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17">
@@ -1560,19 +1676,19 @@
         <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D17" s="0">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="F17" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="G17" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18">
@@ -1583,19 +1699,19 @@
         <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D18" s="0">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="F18" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="G18" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19">
@@ -1606,19 +1722,19 @@
         <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D19" s="0">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="F19" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="G19" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20">
@@ -1629,19 +1745,19 @@
         <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D20" s="0">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="F20" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="G20" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21">
@@ -1652,19 +1768,19 @@
         <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D21" s="0">
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="F21" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="G21" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22">
@@ -1675,19 +1791,19 @@
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D22" s="0">
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="F22" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="G22" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23">
@@ -1698,19 +1814,19 @@
         <v>23</v>
       </c>
       <c r="C23" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D23" s="0">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="F23" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="G23" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24">
@@ -1721,19 +1837,19 @@
         <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D24" s="0">
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="F24" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="G24" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25">
@@ -1744,19 +1860,19 @@
         <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D25" s="0">
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="F25" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="G25" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26">
@@ -1767,19 +1883,19 @@
         <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D26" s="0">
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="F26" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="G26" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27">
@@ -1790,19 +1906,19 @@
         <v>27</v>
       </c>
       <c r="C27" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D27" s="0">
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="F27" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G27" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28">
@@ -1813,19 +1929,19 @@
         <v>28</v>
       </c>
       <c r="C28" t="s">
+        <v>85</v>
+      </c>
+      <c r="D28" s="0">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>87</v>
+      </c>
+      <c r="F28" t="s">
+        <v>49</v>
+      </c>
+      <c r="G28" t="s">
         <v>77</v>
-      </c>
-      <c r="D28" s="0">
-        <v>1</v>
-      </c>
-      <c r="E28" t="s">
-        <v>79</v>
-      </c>
-      <c r="F28" t="s">
-        <v>45</v>
-      </c>
-      <c r="G28" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="29">
@@ -1833,22 +1949,22 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C29" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D29" s="0">
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="F29" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="G29" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30">
@@ -1856,22 +1972,22 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C30" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D30" s="0">
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="F30" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="G30" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31">
@@ -1879,22 +1995,22 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C31" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D31" s="0">
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="F31" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="G31" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1913,19 +2029,19 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="F1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="G1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2">
@@ -1933,22 +2049,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D2" s="0">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G2" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3">
@@ -1959,19 +2075,19 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D3" s="0">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="F3" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G3" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4">
@@ -1982,19 +2098,19 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D4" s="0">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="F4" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="G4" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5">
@@ -2005,19 +2121,19 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D5" s="0">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="F5" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G5" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6">
@@ -2028,19 +2144,19 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D6" s="0">
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G6" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7">
@@ -2051,19 +2167,19 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D7" s="0">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="F7" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G7" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8">
@@ -2074,19 +2190,19 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D8" s="0">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="F8" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G8" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9">
@@ -2097,19 +2213,19 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D9" s="0">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="F9" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="G9" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10">
@@ -2120,19 +2236,19 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D10" s="0">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="F10" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="G10" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11">
@@ -2143,19 +2259,19 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D11" s="0">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="F11" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="G11" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12">
@@ -2166,19 +2282,19 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D12" s="0">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="F12" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="G12" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13">
@@ -2189,19 +2305,19 @@
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D13" s="0">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="F13" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="G13" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14">
@@ -2212,19 +2328,19 @@
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D14" s="0">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="F14" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="G14" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15">
@@ -2235,19 +2351,19 @@
         <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D15" s="0">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="F15" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="G15" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16">
@@ -2258,19 +2374,19 @@
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D16" s="0">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="F16" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="G16" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17">
@@ -2281,19 +2397,19 @@
         <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D17" s="0">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="F17" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="G17" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18">
@@ -2304,19 +2420,19 @@
         <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D18" s="0">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="F18" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="G18" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19">
@@ -2327,19 +2443,19 @@
         <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D19" s="0">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="F19" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="G19" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20">
@@ -2350,19 +2466,19 @@
         <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D20" s="0">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="F20" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="G20" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21">
@@ -2373,19 +2489,19 @@
         <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D21" s="0">
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="F21" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="G21" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22">
@@ -2396,19 +2512,19 @@
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D22" s="0">
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="F22" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="G22" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23">
@@ -2419,19 +2535,19 @@
         <v>23</v>
       </c>
       <c r="C23" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D23" s="0">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="F23" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="G23" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24">
@@ -2442,19 +2558,19 @@
         <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D24" s="0">
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="F24" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="G24" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25">
@@ -2465,19 +2581,19 @@
         <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D25" s="0">
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="F25" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="G25" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26">
@@ -2488,19 +2604,19 @@
         <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D26" s="0">
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="F26" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="G26" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27">
@@ -2508,22 +2624,22 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="C27" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D27" s="0">
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="F27" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="G27" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28">
@@ -2531,22 +2647,22 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="C28" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D28" s="0">
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="F28" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="G28" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29">
@@ -2554,22 +2670,22 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C29" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D29" s="0">
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="F29" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="G29" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30">
@@ -2577,22 +2693,22 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C30" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D30" s="0">
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="F30" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="G30" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31">
@@ -2600,22 +2716,22 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C31" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D31" s="0">
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="F31" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="G31" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2634,19 +2750,19 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="F1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="G1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2">
@@ -2657,19 +2773,19 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D2" s="0">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3">
@@ -2680,19 +2796,19 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D3" s="0">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="F3" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="G3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4">
@@ -2703,19 +2819,19 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D4" s="0">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="F4" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G4" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5">
@@ -2726,19 +2842,19 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D5" s="0">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="F5" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G5" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6">
@@ -2749,19 +2865,19 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D6" s="0">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G6" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7">
@@ -2772,19 +2888,19 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D7" s="0">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="F7" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G7" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8">
@@ -2795,19 +2911,19 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D8" s="0">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="F8" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G8" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9">
@@ -2818,19 +2934,19 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D9" s="0">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="F9" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="G9" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10">
@@ -2841,19 +2957,19 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D10" s="0">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="F10" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="G10" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11">
@@ -2864,19 +2980,19 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D11" s="0">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="F11" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="G11" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12">
@@ -2887,19 +3003,19 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D12" s="0">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="F12" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="G12" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13">
@@ -2910,19 +3026,19 @@
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D13" s="0">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="F13" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="G13" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14">
@@ -2933,19 +3049,19 @@
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D14" s="0">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="F14" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="G14" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15">
@@ -2956,19 +3072,19 @@
         <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D15" s="0">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="F15" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="G15" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16">
@@ -2979,19 +3095,19 @@
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D16" s="0">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="F16" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="G16" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17">
@@ -3002,19 +3118,19 @@
         <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D17" s="0">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="F17" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="G17" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18">
@@ -3025,19 +3141,19 @@
         <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D18" s="0">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="F18" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="G18" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19">
@@ -3048,19 +3164,19 @@
         <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D19" s="0">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="F19" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="G19" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20">
@@ -3071,19 +3187,19 @@
         <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D20" s="0">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="F20" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="G20" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21">
@@ -3094,19 +3210,19 @@
         <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D21" s="0">
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="F21" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="G21" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22">
@@ -3117,19 +3233,19 @@
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D22" s="0">
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="F22" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="G22" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23">
@@ -3140,19 +3256,19 @@
         <v>23</v>
       </c>
       <c r="C23" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D23" s="0">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="F23" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="G23" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24">
@@ -3163,19 +3279,19 @@
         <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D24" s="0">
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="F24" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="G24" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25">
@@ -3186,19 +3302,19 @@
         <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D25" s="0">
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="F25" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="G25" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26">
@@ -3209,19 +3325,19 @@
         <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D26" s="0">
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F26" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G26" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27">
@@ -3229,22 +3345,22 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="C27" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D27" s="0">
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="F27" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="G27" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28">
@@ -3252,22 +3368,22 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="C28" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D28" s="0">
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="F28" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="G28" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29">
@@ -3275,22 +3391,22 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C29" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D29" s="0">
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="F29" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="G29" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30">
@@ -3298,22 +3414,22 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C30" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D30" s="0">
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="F30" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="G30" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31">
@@ -3321,22 +3437,22 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C31" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D31" s="0">
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F31" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="G31" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32">
@@ -3344,22 +3460,22 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="C32" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D32" s="0">
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F32" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="G32" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
     </row>
     <row r="33">
@@ -3367,22 +3483,22 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="C33" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D33" s="0">
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F33" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="G33" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>